<commit_message>
excel data saved to db
</commit_message>
<xml_diff>
--- a/env/src/InvoiceData.xlsx
+++ b/env/src/InvoiceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abeeshek\Desktop\Invoice management system project\Digitization of Invoice\env\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E77B9C-DC73-4BBF-BCD8-E8F790EB8577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DDC0A7-FBB3-4871-8D49-DD8A60A2CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4284" yWindow="3996" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="invoices" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Total</t>
   </si>
@@ -96,7 +96,34 @@
     <t>July 5th, 2021</t>
   </si>
   <si>
-    <t>Sharpner</t>
+    <t>to</t>
+  </si>
+  <si>
+    <t>invoice_type</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>unit_price</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -587,10 +614,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C728E9CD-9D03-4FCD-8DDF-9E799BEBBF3B}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,81 +626,68 @@
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>8264829129</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
       </c>
       <c r="I2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>200</v>
-      </c>
-      <c r="I3">
-        <v>1200</v>
+      <c r="J2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>